<commit_message>
Added some data and data generation notebooks
</commit_message>
<xml_diff>
--- a/Data/widom_lg_data.xlsx
+++ b/Data/widom_lg_data.xlsx
@@ -456,14 +456,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>-1.91824273031694*(sqrt(0.00151790300813824/u**2 + u**(-3)) - 0.0389602747441318/u)**0.333333333333333 + 1.91824273031694/(u*(sqrt(0.00151790300813824/u**2 + u**(-3)) - 0.0389602747441318/u)**0.333333333333333)</t>
+          <t>0.0160865304302357</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>11.03896551724138</v>
+        <v>6.213793103448275</v>
       </c>
       <c r="D2" t="n">
-        <v>0.55</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3">
@@ -472,14 +472,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-0.650295723425693*(sqrt(u**(-2) + 4.89745944291399e-7/u**3) - 1/u)**0.333333333333333 + 0.00512587306552419/(u*(sqrt(u**(-2) + 4.89745944291399e-7/u**3) - 1/u)**0.333333333333333)</t>
+          <t>0.0180905253988772</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.01</v>
+        <v>5.524482758620689</v>
       </c>
       <c r="D3" t="n">
-        <v>0.55</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="4">
@@ -488,14 +488,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>-2.24906110678856*(sqrt(0.00020403242840896/u**2 + u**(-3)) - 0.0142839920333554/u)**0.333333333333333 + 2.24906110678856/(u*(sqrt(0.00020403242840896/u**2 + u**(-3)) - 0.0142839920333554/u)**0.333333333333333)</t>
+          <t>0.321429615119815</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>15.1748275862069</v>
+        <v>2.077931034482758</v>
       </c>
       <c r="D4" t="n">
-        <v>0.325</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -504,14 +504,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>-1.59085027507341*(sqrt(0.00926333924848622/u**2 + u**(-3)) - 0.0962462427759454/u)**0.333333333333333 + 1.59085027507341/(u*(sqrt(0.00926333924848622/u**2 + u**(-3)) - 0.0962462427759454/u)**0.333333333333333)</t>
+          <t>0.0899293642567526</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>7.592413793103447</v>
+        <v>11.03896551724138</v>
       </c>
       <c r="D5" t="n">
-        <v>0.775</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -520,14 +520,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>-2.29957517315949*(sqrt(0.00101544813491639/u**2 + u**(-3)) - 0.0318660969514057/u)**0.333333333333333 + 2.29957517315949/(u*(sqrt(0.00101544813491639/u**2 + u**(-3)) - 0.0318660969514057/u)**0.333333333333333)</t>
+          <t>0.118726984031536</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>15.86413793103448</v>
+        <v>8.281724137931034</v>
       </c>
       <c r="D6" t="n">
-        <v>0.775</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -536,11 +536,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>-2.49141053156271*(sqrt(1.04536566837411e-5/u**2 + u**(-3)) - 0.00323321151237297/u)**0.333333333333333 + 2.49141053156271/(u*(sqrt(1.04536566837411e-5/u**2 + u**(-3)) - 0.00323321151237297/u)**0.333333333333333)</t>
+          <t>0.00724809311535268</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>18.62137931034483</v>
+        <v>13.79620689655172</v>
       </c>
       <c r="D7" t="n">
         <v>0.1</v>
@@ -552,14 +552,14 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>-1.51691610933453*(sqrt(0.000205196820814356/u**2 + u**(-3)) - 0.0143246926952852/u)**0.333333333333333 + 1.51691610933453/(u*(sqrt(0.000205196820814356/u**2 + u**(-3)) - 0.0143246926952852/u)**0.333333333333333)</t>
+          <t>0.0602780649065077</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>6.903103448275861</v>
+        <v>16.55344827586207</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -568,14 +568,14 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>-1.85738662035433*(sqrt(0.00365703853766044/u**2 + u**(-3)) - 0.0604734531646774/u)**0.333333333333333 + 1.85738662035433/(u*(sqrt(0.00365703853766044/u**2 + u**(-3)) - 0.0604734531646774/u)**0.333333333333333)</t>
+          <t>0.0610547285512734</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>10.34965517241379</v>
+        <v>8.97103448275862</v>
       </c>
       <c r="D9" t="n">
-        <v>0.775</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="10">
@@ -584,14 +584,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>-2.53710396943526*(sqrt(9.90095625976641e-5/u**2 + u**(-3)) - 0.00995035489807595/u)**0.333333333333333 + 2.53710396943526/(u*(sqrt(9.90095625976641e-5/u**2 + u**(-3)) - 0.00995035489807595/u)**0.333333333333333)</t>
+          <t>0.0398202631187896</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>19.31068965517241</v>
+        <v>13.79620689655172</v>
       </c>
       <c r="D10" t="n">
-        <v>0.325</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="11">
@@ -600,14 +600,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>-0.960423757048652*(sqrt(0.00318539022711856/u**2 + u**(-3)) - 0.0564392613977058/u)**0.333333333333333 + 0.960423757048652/(u*(sqrt(0.00318539022711856/u**2 + u**(-3)) - 0.0564392613977058/u)**0.333333333333333)</t>
+          <t>0.0204810427736302</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2.767241379310344</v>
+        <v>15.86413793103448</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="12">
@@ -616,14 +616,14 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>-0.960423757048652*(sqrt(0.318539022711856/u**2 + u**(-3)) - 0.564392613977058/u)**0.333333333333333 + 0.960423757048652/(u*(sqrt(0.318539022711856/u**2 + u**(-3)) - 0.564392613977058/u)**0.333333333333333)</t>
+          <t>0.0274896133404174</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2.767241379310344</v>
+        <v>20</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="13">
@@ -632,11 +632,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>-1.26953697777222*(sqrt(0.000597128607704872/u**2 + u**(-3)) - 0.0244362150855011/u)**0.333333333333333 + 1.26953697777222/(u*(sqrt(0.000597128607704872/u**2 + u**(-3)) - 0.0244362150855011/u)**0.333333333333333)</t>
+          <t>0.213896299504187</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4.835172413793103</v>
+        <v>0.01</v>
       </c>
       <c r="D13" t="n">
         <v>0.1</v>
@@ -648,14 +648,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>-2.03450126623181*(sqrt(3.52526867362105e-5/u**2 + u**(-3)) - 0.0059373973032138/u)**0.333333333333333 + 2.03450126623181/(u*(sqrt(3.52526867362105e-5/u**2 + u**(-3)) - 0.0059373973032138/u)**0.333333333333333)</t>
+          <t>0.0856878273322369</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>12.41758620689655</v>
+        <v>8.97103448275862</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="15">
@@ -664,14 +664,14 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>-2.09020705128496*(sqrt(0.00180055985407291/u**2 + u**(-3)) - 0.0424330043017568/u)**0.333333333333333 + 2.09020705128496/(u*(sqrt(0.00180055985407291/u**2 + u**(-3)) - 0.0424330043017568/u)**0.333333333333333)</t>
+          <t>0.00658967213612616</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>13.10689655172414</v>
+        <v>15.1748275862069</v>
       </c>
       <c r="D15" t="n">
-        <v>0.775</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16">
@@ -680,14 +680,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>-1.91824273031694*(sqrt(0.000530011587552401/u**2 + u**(-3)) - 0.0230219805306234/u)**0.333333333333333 + 1.91824273031694/(u*(sqrt(0.000530011587552401/u**2 + u**(-3)) - 0.0230219805306234/u)**0.333333333333333)</t>
+          <t>0.0622175303166177</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>11.03896551724138</v>
+        <v>12.41758620689655</v>
       </c>
       <c r="D16" t="n">
-        <v>0.325</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="17">
@@ -696,14 +696,14 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>-1.91824273031694*(sqrt(0.00301385287359679/u**2 + u**(-3)) - 0.0548985689576403/u)**0.333333333333333 + 1.91824273031694/(u*(sqrt(0.00301385287359679/u**2 + u**(-3)) - 0.0548985689576403/u)**0.333333333333333)</t>
+          <t>0.0874369710638688</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>11.03896551724138</v>
+        <v>6.213793103448275</v>
       </c>
       <c r="D17" t="n">
-        <v>0.775</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="18">
@@ -712,14 +712,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>-2.03450126623181*(sqrt(0.00352526867362105/u**2 + u**(-3)) - 0.059373973032138/u)**0.333333333333333 + 2.03450126623181/(u*(sqrt(0.00352526867362105/u**2 + u**(-3)) - 0.059373973032138/u)**0.333333333333333)</t>
+          <t>0.0131680345315752</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>12.41758620689655</v>
+        <v>7.592413793103447</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19">
@@ -728,11 +728,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>-1.97722666564972*(sqrt(4.18409228964219e-5/u**2 + u**(-3)) - 0.00646845599014339/u)**0.333333333333333 + 1.97722666564972/(u*(sqrt(4.18409228964219e-5/u**2 + u**(-3)) - 0.00646845599014339/u)**0.333333333333333)</t>
+          <t>0.00805267437099078</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>11.72827586206896</v>
+        <v>12.41758620689655</v>
       </c>
       <c r="D19" t="n">
         <v>0.1</v>
@@ -744,11 +744,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>-1.85738662035433*(sqrt(0.00184183834779152/u**2 + u**(-3)) - 0.042916644181384/u)**0.333333333333333 + 1.85738662035433/(u*(sqrt(0.00184183834779152/u**2 + u**(-3)) - 0.042916644181384/u)**0.333333333333333)</t>
+          <t>0.0468077715263697</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>10.34965517241379</v>
+        <v>11.72827586206896</v>
       </c>
       <c r="D20" t="n">
         <v>0.55</v>
@@ -760,14 +760,14 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>-1.66149773176002*(sqrt(0.000118834212448567/u**2 + u**(-3)) - 0.0109011106061982/u)**0.333333333333333 + 1.66149773176002/(u*(sqrt(0.000118834212448567/u**2 + u**(-3)) - 0.0109011106061982/u)**0.333333333333333)</t>
+          <t>0.0469305391119882</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>8.281724137931034</v>
+        <v>6.903103448275861</v>
       </c>
       <c r="D21" t="n">
-        <v>0.1</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="22">
@@ -776,14 +776,14 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>-1.17556540566168*(sqrt(0.0947238246557862/u**2 + u**(-3)) - 0.307772358498593/u)**0.333333333333333 + 1.17556540566168/(u*(sqrt(0.0947238246557862/u**2 + u**(-3)) - 0.307772358498593/u)**0.333333333333333)</t>
+          <t>0.00905814658382476</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>4.145862068965517</v>
+        <v>11.03896551724138</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23">
@@ -792,14 +792,14 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>-2.09020705128496*(sqrt(0.000316643720435299/u**2 + u**(-3)) - 0.0177944856749303/u)**0.333333333333333 + 2.09020705128496/(u*(sqrt(0.000316643720435299/u**2 + u**(-3)) - 0.0177944856749303/u)**0.333333333333333)</t>
+          <t>0.0111454431729087</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>13.10689655172414</v>
+        <v>8.97103448275862</v>
       </c>
       <c r="D23" t="n">
-        <v>0.325</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="24">
@@ -808,11 +808,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>-0.960423757048652*(sqrt(0.0963580543703365/u**2 + u**(-3)) - 0.310415937687382/u)**0.333333333333333 + 0.960423757048652/(u*(sqrt(0.0963580543703365/u**2 + u**(-3)) - 0.310415937687382/u)**0.333333333333333)</t>
+          <t>0.319612667777994</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2.767241379310344</v>
+        <v>0.6993103448275861</v>
       </c>
       <c r="D24" t="n">
         <v>0.55</v>
@@ -824,14 +824,14 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>-1.59085027507341*(sqrt(0.00466540707207839/u**2 + u**(-3)) - 0.0683037851958322/u)**0.333333333333333 + 1.59085027507341/(u*(sqrt(0.00466540707207839/u**2 + u**(-3)) - 0.0683037851958322/u)**0.333333333333333)</t>
+          <t>0.247622727361371</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>7.592413793103447</v>
+        <v>0.6993103448275861</v>
       </c>
       <c r="D25" t="n">
-        <v>0.55</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="26">
@@ -840,14 +840,14 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>-1.79446787169031*(sqrt(7.48731123015435e-5/u**2 + u**(-3)) - 0.00865292507199406/u)**0.333333333333333 + 1.79446787169031/(u*(sqrt(7.48731123015435e-5/u**2 + u**(-3)) - 0.00865292507199406/u)**0.333333333333333)</t>
+          <t>0.0431737828325296</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>9.660344827586206</v>
+        <v>17.93206896551724</v>
       </c>
       <c r="D26" t="n">
-        <v>0.1</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="27">
@@ -856,14 +856,14 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>-0.832252172217603*(sqrt(0.451870291735073/u**2 + u**(-3)) - 0.672212980933181/u)**0.333333333333333 + 0.832252172217603/(u*(sqrt(0.451870291735073/u**2 + u**(-3)) - 0.672212980933181/u)**0.333333333333333)</t>
+          <t>0.0427033197092875</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>2.077931034482758</v>
+        <v>7.592413793103447</v>
       </c>
       <c r="D27" t="n">
-        <v>0.775</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="28">
@@ -872,11 +872,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>-2.58198889747161*(sqrt(0.00050677734375/u**2 + u**(-3)) - 0.0225117156998306/u)**0.333333333333333 + 2.58198889747161/(u*(sqrt(0.00050677734375/u**2 + u**(-3)) - 0.0225117156998306/u)**0.333333333333333)</t>
+          <t>0.174185902873399</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>20</v>
+        <v>4.145862068965517</v>
       </c>
       <c r="D28" t="n">
         <v>0.775</v>
@@ -888,14 +888,14 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>-2.49141053156271*(sqrt(0.000110416748722015/u**2 + u**(-3)) - 0.0105079374152121/u)**0.333333333333333 + 2.49141053156271/(u*(sqrt(0.000110416748722015/u**2 + u**(-3)) - 0.0105079374152121/u)**0.333333333333333)</t>
+          <t>0.0978604261077026</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>18.62137931034483</v>
+        <v>5.524482758620689</v>
       </c>
       <c r="D29" t="n">
-        <v>0.325</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="30">
@@ -904,14 +904,14 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>-2.19738611698682*(sqrt(2.22076063557366e-5/u**2 + u**(-3)) - 0.00471249470617598/u)**0.333333333333333 + 2.19738611698682/(u*(sqrt(2.22076063557366e-5/u**2 + u**(-3)) - 0.00471249470617598/u)**0.333333333333333)</t>
+          <t>0.0261581444148770</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>14.48551724137931</v>
+        <v>12.41758620689655</v>
       </c>
       <c r="D30" t="n">
-        <v>0.1</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="31">
@@ -920,14 +920,14 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>-1.97722666564972*(sqrt(0.000441944748093456/u**2 + u**(-3)) - 0.021022481967966/u)**0.333333333333333 + 1.97722666564972/(u*(sqrt(0.000441944748093456/u**2 + u**(-3)) - 0.021022481967966/u)**0.333333333333333)</t>
+          <t>0.0628785483162015</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>11.72827586206896</v>
+        <v>15.86413793103448</v>
       </c>
       <c r="D31" t="n">
-        <v>0.325</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -936,14 +936,14 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>-1.35701667376402*(sqrt(0.000400339926650359/u**2 + u**(-3)) - 0.020008496361555/u)**0.333333333333333 + 1.35701667376402/(u*(sqrt(0.000400339926650359/u**2 + u**(-3)) - 0.020008496361555/u)**0.333333333333333)</t>
+          <t>0.0772782576713545</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>5.524482758620689</v>
+        <v>4.145862068965517</v>
       </c>
       <c r="D32" t="n">
-        <v>0.1</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="33">
@@ -952,11 +952,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>-1.97722666564972*(sqrt(0.00126568791761676/u**2 + u**(-3)) - 0.0355765079457886/u)**0.333333333333333 + 1.97722666564972/(u*(sqrt(0.00126568791761676/u**2 + u**(-3)) - 0.0355765079457886/u)**0.333333333333333)</t>
+          <t>0.0332035916855847</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>11.72827586206896</v>
+        <v>16.55344827586207</v>
       </c>
       <c r="D33" t="n">
         <v>0.55</v>
@@ -968,14 +968,14 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>-1.07339829888349*(sqrt(0.0172639955155382/u**2 + u**(-3)) - 0.131392524580123/u)**0.333333333333333 + 1.07339829888349/(u*(sqrt(0.0172639955155382/u**2 + u**(-3)) - 0.131392524580123/u)**0.333333333333333)</t>
+          <t>0.0295221255639259</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>3.45655172413793</v>
+        <v>18.62137931034483</v>
       </c>
       <c r="D34" t="n">
-        <v>0.325</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="35">
@@ -984,14 +984,14 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>-2.44486325217569*(sqrt(0.000703098184379026/u**2 + u**(-3)) - 0.0265159986494762/u)**0.333333333333333 + 2.44486325217569/(u*(sqrt(0.000703098184379026/u**2 + u**(-3)) - 0.0265159986494762/u)**0.333333333333333)</t>
+          <t>0.0847450935780748</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>17.93206896551724</v>
+        <v>11.72827586206896</v>
       </c>
       <c r="D35" t="n">
-        <v>0.775</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1000,14 +1000,14 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>-0.545696441530553*(sqrt(u**(-2) + 1.40258601797063e-6/u**3) - 1/u)**0.333333333333333 + 0.00610840218049453/(u*(sqrt(u**(-2) + 1.40258601797063e-6/u**3) - 1/u)**0.333333333333333)</t>
+          <t>0.0400998209000983</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.01</v>
+        <v>19.31068965517241</v>
       </c>
       <c r="D36" t="n">
-        <v>0.325</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="37">
@@ -1016,14 +1016,14 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>-1.26953697777222*(sqrt(0.0597128607704872/u**2 + u**(-3)) - 0.244362150855011/u)**0.333333333333333 + 1.26953697777222/(u*(sqrt(0.0597128607704872/u**2 + u**(-3)) - 0.244362150855011/u)**0.333333333333333)</t>
+          <t>0.0467562905399777</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>4.835172413793103</v>
+        <v>16.55344827586207</v>
       </c>
       <c r="D37" t="n">
-        <v>1</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="38">
@@ -1032,14 +1032,14 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>-1.66149773176002*(sqrt(0.00713747988519204/u**2 + u**(-3)) - 0.084483607198036/u)**0.333333333333333 + 1.66149773176002/(u*(sqrt(0.00713747988519204/u**2 + u**(-3)) - 0.084483607198036/u)**0.333333333333333)</t>
+          <t>0.0719501443247458</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>8.281724137931034</v>
+        <v>7.592413793103447</v>
       </c>
       <c r="D38" t="n">
-        <v>0.775</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="39">
@@ -1048,14 +1048,14 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>-1.79446787169031*(sqrt(0.00449706630761146/u**2 + u**(-3)) - 0.067060169307954/u)**0.333333333333333 + 1.79446787169031/(u*(sqrt(0.00449706630761146/u**2 + u**(-3)) - 0.067060169307954/u)**0.333333333333333)</t>
+          <t>0.366274635959563</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>9.660344827586206</v>
+        <v>1.388620689655172</v>
       </c>
       <c r="D39" t="n">
-        <v>0.775</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -1064,7 +1064,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>-2.24906110678856*(sqrt(0.00058432955828365/u**2 + u**(-3)) - 0.0241729095949091/u)**0.333333333333333 + 2.24906110678856/(u*(sqrt(0.00058432955828365/u**2 + u**(-3)) - 0.0241729095949091/u)**0.333333333333333)</t>
+          <t>0.0362129394042180</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1080,14 +1080,14 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>-2.53710396943526*(sqrt(9.37368639977885e-6/u**2 + u**(-3)) - 0.00306164766094645/u)**0.333333333333333 + 2.53710396943526/(u*(sqrt(9.37368639977885e-6/u**2 + u**(-3)) - 0.00306164766094645/u)**0.333333333333333)</t>
+          <t>0.318080696503262</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>19.31068965517241</v>
+        <v>0.01</v>
       </c>
       <c r="D41" t="n">
-        <v>0.1</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="42">
@@ -1096,14 +1096,14 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>-2.24906110678856*(sqrt(0.00193166796126826/u**2 + u**(-3)) - 0.0439507447180166/u)**0.333333333333333 + 2.24906110678856/(u*(sqrt(0.00193166796126826/u**2 + u**(-3)) - 0.0439507447180166/u)**0.333333333333333)</t>
+          <t>0.00579942291498248</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>15.1748275862069</v>
+        <v>17.24275862068966</v>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="43">
@@ -1112,14 +1112,14 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>-1.35701667376402*(sqrt(0.0121102827811733/u**2 + u**(-3)) - 0.110046729988552/u)**0.333333333333333 + 1.35701667376402/(u*(sqrt(0.0121102827811733/u**2 + u**(-3)) - 0.110046729988552/u)**0.333333333333333)</t>
+          <t>0.372014032551493</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>5.524482758620689</v>
+        <v>0.6993103448275861</v>
       </c>
       <c r="D43" t="n">
-        <v>0.55</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="44">
@@ -1128,14 +1128,14 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>-2.29957517315949*(sqrt(0.000511422369718556/u**2 + u**(-3)) - 0.0226146494493847/u)**0.333333333333333 + 2.29957517315949/(u*(sqrt(0.000511422369718556/u**2 + u**(-3)) - 0.0226146494493847/u)**0.333333333333333)</t>
+          <t>0.0168275890450742</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>15.86413793103448</v>
+        <v>19.31068965517241</v>
       </c>
       <c r="D44" t="n">
-        <v>0.55</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="45">
@@ -1144,14 +1144,14 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>-1.51691610933453*(sqrt(0.00216739141985164/u**2 + u**(-3)) - 0.0465552512596768/u)**0.333333333333333 + 1.51691610933453/(u*(sqrt(0.00216739141985164/u**2 + u**(-3)) - 0.0465552512596768/u)**0.333333333333333)</t>
+          <t>0.0415802234829786</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>6.903103448275861</v>
+        <v>18.62137931034483</v>
       </c>
       <c r="D45" t="n">
-        <v>0.325</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="46">
@@ -1160,14 +1160,14 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>-2.39741239816944*(sqrt(0.000139075377988964/u**2 + u**(-3)) - 0.0117930224280701/u)**0.333333333333333 + 2.39741239816944/(u*(sqrt(0.000139075377988964/u**2 + u**(-3)) - 0.0117930224280701/u)**0.333333333333333)</t>
+          <t>0.414155067460626</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>17.24275862068966</v>
+        <v>0.6993103448275861</v>
       </c>
       <c r="D46" t="n">
-        <v>0.325</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -1176,14 +1176,14 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>-1.85738662035433*(sqrt(6.08872181088106e-5/u**2 + u**(-3)) - 0.00780302621479709/u)**0.333333333333333 + 1.85738662035433/(u*(sqrt(6.08872181088106e-5/u**2 + u**(-3)) - 0.00780302621479709/u)**0.333333333333333)</t>
+          <t>0.0658363076876488</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>10.34965517241379</v>
+        <v>11.72827586206896</v>
       </c>
       <c r="D47" t="n">
-        <v>0.1</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="48">
@@ -1192,11 +1192,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>-2.58198889747161*(sqrt(8.4375e-6/u**2 + u**(-3)) - 0.00290473750965556/u)**0.333333333333333 + 2.58198889747161/(u*(sqrt(8.4375e-6/u**2 + u**(-3)) - 0.00290473750965556/u)**0.333333333333333)</t>
+          <t>0.0240867289457211</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>20</v>
+        <v>4.145862068965517</v>
       </c>
       <c r="D48" t="n">
         <v>0.1</v>
@@ -1208,14 +1208,14 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>-1.51691610933453*(sqrt(0.0123246340501623/u**2 + u**(-3)) - 0.11101636838846/u)**0.333333333333333 + 1.51691610933453/(u*(sqrt(0.0123246340501623/u**2 + u**(-3)) - 0.11101636838846/u)**0.333333333333333)</t>
+          <t>0.178277882794008</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>6.903103448275861</v>
+        <v>2.767241379310344</v>
       </c>
       <c r="D49" t="n">
-        <v>0.775</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="50">
@@ -1224,14 +1224,14 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>-2.58198889747161*(sqrt(0.000255234375/u**2 + u**(-3)) - 0.0159760563031056/u)**0.333333333333333 + 2.58198889747161/(u*(sqrt(0.000255234375/u**2 + u**(-3)) - 0.0159760563031056/u)**0.333333333333333)</t>
+          <t>0.0276927003145796</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>20</v>
+        <v>11.72827586206896</v>
       </c>
       <c r="D50" t="n">
-        <v>0.55</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="51">
@@ -1240,14 +1240,14 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>-1.72926135317545*(sqrt(0.00934923755211874/u**2 + u**(-3)) - 0.0966914554245552/u)**0.333333333333333 + 1.72926135317546/(u*(sqrt(0.00934923755211874/u**2 + u**(-3)) - 0.0966914554245552/u)**0.333333333333333)</t>
+          <t>0.0306552423088085</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>8.97103448275862</v>
+        <v>17.93206896551724</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="52">
@@ -1256,11 +1256,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>-1.85738662035433*(sqrt(0.00608872181088106/u**2 + u**(-3)) - 0.0780302621479709/u)**0.333333333333333 + 1.85738662035433/(u*(sqrt(0.00608872181088106/u**2 + u**(-3)) - 0.0780302621479709/u)**0.333333333333333)</t>
+          <t>0.0499377332097978</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>10.34965517241379</v>
+        <v>20</v>
       </c>
       <c r="D52" t="n">
         <v>1</v>
@@ -1272,14 +1272,14 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>-1.85738662035433*(sqrt(0.000643121241274312/u**2 + u**(-3)) - 0.0253598351980905/u)**0.333333333333333 + 1.85738662035433/(u*(sqrt(0.000643121241274312/u**2 + u**(-3)) - 0.0253598351980905/u)**0.333333333333333)</t>
+          <t>0.0578828885213668</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>10.34965517241379</v>
+        <v>17.24275862068966</v>
       </c>
       <c r="D53" t="n">
-        <v>0.325</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -1288,14 +1288,14 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>-0.650295723425693*(sqrt(u**(-2) + 0.167486846834147/u**3) - 1/u)**0.333333333333333 + 0.358457606099416/(u*(sqrt(u**(-2) + 0.167486846834147/u**3) - 1/u)**0.333333333333333)</t>
+          <t>0.200791549440062</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.6993103448275861</v>
+        <v>3.45655172413793</v>
       </c>
       <c r="D54" t="n">
-        <v>0.55</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="55">
@@ -1304,14 +1304,14 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>-2.49141053156271*(sqrt(0.0006278727545672/u**2 + u**(-3)) - 0.0250573892208905/u)**0.333333333333333 + 2.49141053156271/(u*(sqrt(0.0006278727545672/u**2 + u**(-3)) - 0.0250573892208905/u)**0.333333333333333)</t>
+          <t>0.127645846300701</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>18.62137931034483</v>
+        <v>4.145862068965517</v>
       </c>
       <c r="D55" t="n">
-        <v>0.775</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="56">
@@ -1320,11 +1320,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>-2.53710396943526*(sqrt(0.000937368639977885/u**2 + u**(-3)) - 0.0306164766094645/u)**0.333333333333333 + 2.53710396943526/(u*(sqrt(0.000937368639977885/u**2 + u**(-3)) - 0.0306164766094645/u)**0.333333333333333)</t>
+          <t>0.0957727861467490</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>19.31068965517241</v>
+        <v>10.34965517241379</v>
       </c>
       <c r="D56" t="n">
         <v>1</v>
@@ -1336,11 +1336,11 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>-1.17556540566168*(sqrt(0.0568934971838816/u**2 + u**(-3)) - 0.238523577836409/u)**0.333333333333333 + 1.17556540566168/(u*(sqrt(0.0568934971838816/u**2 + u**(-3)) - 0.238523577836409/u)**0.333333333333333)</t>
+          <t>0.233849502595008</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>4.145862068965517</v>
+        <v>2.767241379310344</v>
       </c>
       <c r="D57" t="n">
         <v>0.775</v>
@@ -1352,11 +1352,11 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>-1.43918878810811*(sqrt(0.0168980585907913/u**2 + u**(-3)) - 0.129992532827049/u)**0.333333333333333 + 1.43918878810811/(u*(sqrt(0.0168980585907913/u**2 + u**(-3)) - 0.129992532827049/u)**0.333333333333333)</t>
+          <t>0.0926201565294836</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>6.213793103448275</v>
+        <v>8.281724137931034</v>
       </c>
       <c r="D58" t="n">
         <v>0.775</v>
@@ -1368,14 +1368,14 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>-0.680348119140775*(sqrt(0.025208840922476/u**2 + u**(-3)) - 0.158772922510345/u)**0.333333333333333 + 0.680348119140775/(u*(sqrt(0.025208840922476/u**2 + u**(-3)) - 0.158772922510345/u)**0.333333333333333)</t>
+          <t>0.149459265437980</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1.388620689655172</v>
+        <v>3.45655172413793</v>
       </c>
       <c r="D59" t="n">
-        <v>0.1</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="60">
@@ -1384,11 +1384,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>-0.832252172217603*(sqrt(0.752333472191589/u**2 + u**(-3)) - 0.867371588300879/u)**0.333333333333333 + 0.832252172217603/(u*(sqrt(0.752333472191589/u**2 + u**(-3)) - 0.867371588300879/u)**0.333333333333333)</t>
+          <t>0.0801168214923740</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2.077931034482758</v>
+        <v>12.41758620689655</v>
       </c>
       <c r="D60" t="n">
         <v>1</v>
@@ -1400,14 +1400,14 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>-2.34900321241884*(sqrt(1.48812133941955e-5/u**2 + u**(-3)) - 0.0038576175800869/u)**0.333333333333333 + 2.34900321241884/(u*(sqrt(1.48812133941955e-5/u**2 + u**(-3)) - 0.0038576175800869/u)**0.333333333333333)</t>
+          <t>0.110926901025130</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>16.55344827586207</v>
+        <v>4.835172413793103</v>
       </c>
       <c r="D61" t="n">
-        <v>0.1</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="62">
@@ -1416,14 +1416,14 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>-2.19738611698682*(sqrt(0.000234567842132468/u**2 + u**(-3)) - 0.0153156077950719/u)**0.333333333333333 + 2.19738611698682/(u*(sqrt(0.000234567842132468/u**2 + u**(-3)) - 0.0153156077950719/u)**0.333333333333333)</t>
+          <t>0.0509840870943319</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>14.48551724137931</v>
+        <v>15.1748275862069</v>
       </c>
       <c r="D62" t="n">
-        <v>0.325</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="63">
@@ -1432,14 +1432,14 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>-1.07339829888349*(sqrt(0.0981698206534448/u**2 + u**(-3)) - 0.313320635537216/u)**0.333333333333333 + 1.07339829888349/(u*(sqrt(0.0981698206534448/u**2 + u**(-3)) - 0.313320635537216/u)**0.333333333333333)</t>
+          <t>0.0284696847439762</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>3.45655172413793</v>
+        <v>19.31068965517241</v>
       </c>
       <c r="D63" t="n">
-        <v>0.775</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="64">
@@ -1448,14 +1448,14 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>-2.34900321241884*(sqrt(0.000450156705174414/u**2 + u**(-3)) - 0.0212168966904779/u)**0.333333333333333 + 2.34900321241884/(u*(sqrt(0.000450156705174414/u**2 + u**(-3)) - 0.0212168966904779/u)**0.333333333333333)</t>
+          <t>0.0196288028204378</t>
         </is>
       </c>
       <c r="C64" t="n">
         <v>16.55344827586207</v>
       </c>
       <c r="D64" t="n">
-        <v>0.55</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="65">
@@ -1464,11 +1464,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>-1.59085027507341*(sqrt(0.0016290367669034/u**2 + u**(-3)) - 0.040361327615719/u)**0.333333333333333 + 1.59085027507341/(u*(sqrt(0.0016290367669034/u**2 + u**(-3)) - 0.040361327615719/u)**0.333333333333333)</t>
+          <t>0.0224284139871160</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>7.592413793103447</v>
+        <v>14.48551724137931</v>
       </c>
       <c r="D65" t="n">
         <v>0.325</v>
@@ -1480,14 +1480,14 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>-1.79446787169031*(sqrt(0.00748731123015435/u**2 + u**(-3)) - 0.0865292507199406/u)**0.333333333333333 + 1.79446787169031/(u*(sqrt(0.00748731123015435/u**2 + u**(-3)) - 0.0865292507199406/u)**0.333333333333333)</t>
+          <t>0.135755820083289</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>9.660344827586206</v>
+        <v>5.524482758620689</v>
       </c>
       <c r="D66" t="n">
-        <v>1</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="67">
@@ -1496,14 +1496,14 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>-1.66149773176002*(sqrt(0.00359473492656914/u**2 + u**(-3)) - 0.0599561083340901/u)**0.333333333333333 + 1.66149773176002/(u*(sqrt(0.00359473492656914/u**2 + u**(-3)) - 0.0599561083340901/u)**0.333333333333333)</t>
+          <t>0.0206635383184800</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>8.281724137931034</v>
+        <v>4.835172413793103</v>
       </c>
       <c r="D67" t="n">
-        <v>0.55</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="68">
@@ -1512,11 +1512,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>-1.91824273031694*(sqrt(0.00501786118392806/u**2 + u**(-3)) - 0.0708368631711488/u)**0.333333333333333 + 1.91824273031694/(u*(sqrt(0.00501786118392806/u**2 + u**(-3)) - 0.0708368631711488/u)**0.333333333333333)</t>
+          <t>0.246155298351704</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>11.03896551724138</v>
+        <v>3.45655172413793</v>
       </c>
       <c r="D68" t="n">
         <v>1</v>
@@ -1528,11 +1528,11 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>-0.545696441530553*(sqrt(u**(-2) + 0.479666472590102/u**3) - 1/u)**0.333333333333333 + 0.427166883518721/(u*(sqrt(u**(-2) + 0.479666472590102/u**3) - 1/u)**0.333333333333333)</t>
+          <t>0.0235477353466118</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0.6993103448275861</v>
+        <v>13.79620689655172</v>
       </c>
       <c r="D69" t="n">
         <v>0.325</v>
@@ -1544,14 +1544,14 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>-2.03450126623181*(sqrt(0.00106639377377037/u**2 + u**(-3)) - 0.0326556851676759/u)**0.333333333333333 + 2.03450126623181/(u*(sqrt(0.00106639377377037/u**2 + u**(-3)) - 0.0326556851676759/u)**0.333333333333333)</t>
+          <t>0.0556698016369251</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>12.41758620689655</v>
+        <v>17.93206896551724</v>
       </c>
       <c r="D70" t="n">
-        <v>0.55</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -1560,11 +1560,11 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>-1.59085027507341*(sqrt(0.0154228332961269/u**2 + u**(-3)) - 0.124188700356059/u)**0.333333333333333 + 1.59085027507341/(u*(sqrt(0.0154228332961269/u**2 + u**(-3)) - 0.124188700356059/u)**0.333333333333333)</t>
+          <t>0.0536189314734579</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>7.592413793103447</v>
+        <v>18.62137931034483</v>
       </c>
       <c r="D71" t="n">
         <v>1</v>
@@ -1576,11 +1576,11 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>-1.26953697777222*(sqrt(0.00630717091888271/u**2 + u**(-3)) - 0.0794176990278786/u)**0.333333333333333 + 1.26953697777222/(u*(sqrt(0.00630717091888271/u**2 + u**(-3)) - 0.0794176990278786/u)**0.333333333333333)</t>
+          <t>0.0181206362837405</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>4.835172413793103</v>
+        <v>17.93206896551724</v>
       </c>
       <c r="D72" t="n">
         <v>0.325</v>
@@ -1592,14 +1592,14 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>-2.49141053156271*(sqrt(0.00104536566837411/u**2 + u**(-3)) - 0.0323321151237297/u)**0.333333333333333 + 2.49141053156271/(u*(sqrt(0.00104536566837411/u**2 + u**(-3)) - 0.0323321151237297/u)**0.333333333333333)</t>
+          <t>0.0448939288471313</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>18.62137931034483</v>
+        <v>17.24275862068966</v>
       </c>
       <c r="D73" t="n">
-        <v>1</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="74">
@@ -1608,14 +1608,14 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>-2.58198889747161*(sqrt(0.00084375/u**2 + u**(-3)) - 0.0290473750965556/u)**0.333333333333333 + 2.58198889747161/(u*(sqrt(0.00084375/u**2 + u**(-3)) - 0.0290473750965556/u)**0.333333333333333)</t>
+          <t>0.0533966128933417</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>20</v>
+        <v>14.48551724137931</v>
       </c>
       <c r="D74" t="n">
-        <v>1</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="75">
@@ -1624,14 +1624,14 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>-2.44486325217569*(sqrt(1.17061092092242e-5/u**2 + u**(-3)) - 0.00342141918057758/u)**0.333333333333333 + 2.44486325217569/(u*(sqrt(1.17061092092242e-5/u**2 + u**(-3)) - 0.00342141918057758/u)**0.333333333333333)</t>
+          <t>0.112324260215454</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>17.93206896551724</v>
+        <v>2.767241379310344</v>
       </c>
       <c r="D75" t="n">
-        <v>0.1</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="76">
@@ -1640,14 +1640,14 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>-2.49141053156271*(sqrt(0.000316223114683168/u**2 + u**(-3)) - 0.0177826633180513/u)**0.333333333333333 + 2.49141053156271/(u*(sqrt(0.000316223114683168/u**2 + u**(-3)) - 0.0177826633180513/u)**0.333333333333333)</t>
+          <t>0.154945678504179</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>18.62137931034483</v>
+        <v>6.213793103448275</v>
       </c>
       <c r="D76" t="n">
-        <v>0.55</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -1656,14 +1656,14 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>-2.14446628142853*(sqrt(2.57054183757931e-5/u**2 + u**(-3)) - 0.00507005112161536/u)**0.333333333333333 + 2.14446628142853/(u*(sqrt(2.57054183757931e-5/u**2 + u**(-3)) - 0.00507005112161536/u)**0.333333333333333)</t>
+          <t>0.425569122927914</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>13.79620689655172</v>
+        <v>0.01</v>
       </c>
       <c r="D77" t="n">
-        <v>0.1</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="78">
@@ -1672,14 +1672,14 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>-1.79446787169031*(sqrt(0.00226491164712169/u**2 + u**(-3)) - 0.0475910878959674/u)**0.333333333333333 + 1.79446787169031/(u*(sqrt(0.00226491164712169/u**2 + u**(-3)) - 0.0475910878959674/u)**0.333333333333333)</t>
+          <t>0.142484526292082</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>9.660344827586206</v>
+        <v>2.077931034482758</v>
       </c>
       <c r="D78" t="n">
-        <v>0.55</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="79">
@@ -1688,14 +1688,14 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>-1.26953697777222*(sqrt(0.0180631403830724/u**2 + u**(-3)) - 0.134399182970256/u)**0.333333333333333 + 1.26953697777222/(u*(sqrt(0.0180631403830724/u**2 + u**(-3)) - 0.134399182970256/u)**0.333333333333333)</t>
+          <t>0.0744824796090953</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>4.835172413793103</v>
+        <v>10.34965517241379</v>
       </c>
       <c r="D79" t="n">
-        <v>0.55</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="80">
@@ -1704,14 +1704,14 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>-2.39741239816944*(sqrt(0.000790836912706477/u**2 + u**(-3)) - 0.0281218227130902/u)**0.333333333333333 + 2.39741239816944/(u*(sqrt(0.000790836912706477/u**2 + u**(-3)) - 0.0281218227130902/u)**0.333333333333333)</t>
+          <t>0.00690321986040487</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>17.24275862068966</v>
+        <v>14.48551724137931</v>
       </c>
       <c r="D80" t="n">
-        <v>0.775</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="81">
@@ -1720,14 +1720,14 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>-0.832252172217603*(sqrt(0.0075233347219159/u**2 + u**(-3)) - 0.0867371588300879/u)**0.333333333333333 + 0.832252172217603/(u*(sqrt(0.0075233347219159/u**2 + u**(-3)) - 0.0867371588300879/u)**0.333333333333333)</t>
+          <t>0.0313721786228656</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>2.077931034482758</v>
+        <v>10.34965517241379</v>
       </c>
       <c r="D81" t="n">
-        <v>0.1</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="82">
@@ -1736,14 +1736,14 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>-1.43918878810811*(sqrt(0.0281341246048555/u**2 + u**(-3)) - 0.167732300421998/u)**0.333333333333333 + 1.43918878810811/(u*(sqrt(0.0281341246048555/u**2 + u**(-3)) - 0.167732300421998/u)**0.333333333333333)</t>
+          <t>0.00966128633715446</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>6.213793103448275</v>
+        <v>10.34965517241379</v>
       </c>
       <c r="D82" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="83">
@@ -1752,14 +1752,14 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>-1.17556540566168*(sqrt(0.0100052039792674/u**2 + u**(-3)) - 0.100026016512043/u)**0.333333333333333 + 1.17556540566168/(u*(sqrt(0.0100052039792674/u**2 + u**(-3)) - 0.100026016512043/u)**0.333333333333333)</t>
+          <t>0.0567446460553336</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>4.145862068965517</v>
+        <v>9.660344827586206</v>
       </c>
       <c r="D83" t="n">
-        <v>0.325</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="84">
@@ -1768,14 +1768,14 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>-1.72926135317545*(sqrt(9.34923755211874e-5/u**2 + u**(-3)) - 0.00966914554245552/u)**0.333333333333333 + 1.72926135317546/(u*(sqrt(9.34923755211874e-5/u**2 + u**(-3)) - 0.00966914554245552/u)**0.333333333333333)</t>
+          <t>0.0379312828318110</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>8.97103448275862</v>
+        <v>14.48551724137931</v>
       </c>
       <c r="D84" t="n">
-        <v>0.1</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="85">
@@ -1784,14 +1784,14 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>-1.17556540566168*(sqrt(0.000947238246557863/u**2 + u**(-3)) - 0.0307772358498593/u)**0.333333333333333 + 1.17556540566168/(u*(sqrt(0.000947238246557863/u**2 + u**(-3)) - 0.0307772358498593/u)**0.333333333333333)</t>
+          <t>0.0657116237352142</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>4.145862068965517</v>
+        <v>15.1748275862069</v>
       </c>
       <c r="D85" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -1800,14 +1800,14 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>-1.66149773176002*(sqrt(0.0118834212448567/u**2 + u**(-3)) - 0.109011106061982/u)**0.333333333333333 + 1.66149773176002/(u*(sqrt(0.0118834212448567/u**2 + u**(-3)) - 0.109011106061982/u)**0.333333333333333)</t>
+          <t>0.0698965124034789</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>8.281724137931034</v>
+        <v>11.03896551724138</v>
       </c>
       <c r="D86" t="n">
-        <v>1</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="87">
@@ -1816,14 +1816,14 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>-1.72926135317545*(sqrt(0.00561538580474132/u**2 + u**(-3)) - 0.0749358779540303/u)**0.333333333333333 + 1.72926135317546/(u*(sqrt(0.00561538580474132/u**2 + u**(-3)) - 0.0749358779540303/u)**0.333333333333333)</t>
+          <t>0.281102154816828</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>8.97103448275862</v>
+        <v>2.767241379310344</v>
       </c>
       <c r="D87" t="n">
-        <v>0.775</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
@@ -1832,14 +1832,14 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>-1.66149773176002*(sqrt(0.00125518636898799/u**2 + u**(-3)) - 0.0354286094701441/u)**0.333333333333333 + 1.66149773176002/(u*(sqrt(0.00125518636898799/u**2 + u**(-3)) - 0.0354286094701441/u)**0.333333333333333)</t>
+          <t>0.0759613031240484</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>8.281724137931034</v>
+        <v>13.10689655172414</v>
       </c>
       <c r="D88" t="n">
-        <v>0.325</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -1848,11 +1848,11 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>-2.34900321241884*(sqrt(0.00148812133941955/u**2 + u**(-3)) - 0.038576175800869/u)**0.333333333333333 + 2.34900321241884/(u*(sqrt(0.00148812133941955/u**2 + u**(-3)) - 0.038576175800869/u)**0.333333333333333)</t>
+          <t>0.0688095577979265</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>16.55344827586207</v>
+        <v>14.48551724137931</v>
       </c>
       <c r="D89" t="n">
         <v>1</v>
@@ -1864,14 +1864,14 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>-1.72926135317545*(sqrt(0.000987513216442542/u**2 + u**(-3)) - 0.0314247230129804/u)**0.333333333333333 + 1.72926135317546/(u*(sqrt(0.000987513216442542/u**2 + u**(-3)) - 0.0314247230129804/u)**0.333333333333333)</t>
+          <t>0.0419064921477830</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>8.97103448275862</v>
+        <v>13.10689655172414</v>
       </c>
       <c r="D90" t="n">
-        <v>0.325</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="91">
@@ -1880,14 +1880,14 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>-2.14446628142853*(sqrt(0.00154393169119608/u**2 + u**(-3)) - 0.039292896192519/u)**0.333333333333333 + 2.14446628142853/(u*(sqrt(0.00154393169119608/u**2 + u**(-3)) - 0.039292896192519/u)**0.333333333333333)</t>
+          <t>0.0318786596478471</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>13.79620689655172</v>
+        <v>17.24275862068966</v>
       </c>
       <c r="D91" t="n">
-        <v>0.775</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="92">
@@ -1896,11 +1896,11 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>-0.832252172217603*(sqrt(0.227580875337956/u**2 + u**(-3)) - 0.477054373565483/u)**0.333333333333333 + 0.832252172217603/(u*(sqrt(0.227580875337956/u**2 + u**(-3)) - 0.477054373565483/u)**0.333333333333333)</t>
+          <t>0.0442223770229613</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>2.077931034482758</v>
+        <v>12.41758620689655</v>
       </c>
       <c r="D92" t="n">
         <v>0.55</v>
@@ -1912,14 +1912,14 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>-1.43918878810811*(sqrt(0.00851057269296879/u**2 + u**(-3)) - 0.0922527652320991/u)**0.333333333333333 + 1.43918878810811/(u*(sqrt(0.00851057269296879/u**2 + u**(-3)) - 0.0922527652320991/u)**0.333333333333333)</t>
+          <t>0.0487791614508819</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>6.213793103448275</v>
+        <v>15.86413793103448</v>
       </c>
       <c r="D93" t="n">
-        <v>0.55</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="94">
@@ -1928,14 +1928,14 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>-2.03450126623181*(sqrt(0.000372356503651223/u**2 + u**(-3)) - 0.0192965412354448/u)**0.333333333333333 + 2.03450126623181/(u*(sqrt(0.000372356503651223/u**2 + u**(-3)) - 0.0192965412354448/u)**0.333333333333333)</t>
+          <t>0.00537008831169239</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>12.41758620689655</v>
+        <v>18.62137931034483</v>
       </c>
       <c r="D94" t="n">
-        <v>0.325</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="95">
@@ -1944,14 +1944,14 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>-0.832252172217603*(sqrt(0.0794652230002366/u**2 + u**(-3)) - 0.281895766197786/u)**0.333333333333333 + 0.832252172217603/(u*(sqrt(0.0794652230002366/u**2 + u**(-3)) - 0.281895766197786/u)**0.333333333333333)</t>
+          <t>0.152892151892436</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>2.077931034482758</v>
+        <v>4.835172413793103</v>
       </c>
       <c r="D95" t="n">
-        <v>0.325</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="96">
@@ -1960,14 +1960,14 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>-0.729049867913356*(sqrt(u**(-2) + 0.0843534171360325/u**3) - 1/u)**0.333333333333333 + 0.319735944734531/(u*(sqrt(u**(-2) + 0.0843534171360325/u**3) - 1/u)**0.333333333333333)</t>
+          <t>0.0359689070117811</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>0.6993103448275861</v>
+        <v>2.767241379310344</v>
       </c>
       <c r="D96" t="n">
-        <v>0.775</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="97">
@@ -1976,14 +1976,14 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>-2.29957517315949*(sqrt(0.000178575166286025/u**2 + u**(-3)) - 0.0133632019473637/u)**0.333333333333333 + 2.29957517315949/(u*(sqrt(0.000178575166286025/u**2 + u**(-3)) - 0.0133632019473637/u)**0.333333333333333)</t>
+          <t>0.171829122796567</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>15.86413793103448</v>
+        <v>5.524482758620689</v>
       </c>
       <c r="D97" t="n">
-        <v>0.325</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
@@ -1992,11 +1992,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>-0.680348119140775*(sqrt(0.7625674379049/u**2 + u**(-3)) - 0.873251073806898/u)**0.333333333333333 + 0.680348119140775/(u*(sqrt(0.7625674379049/u**2 + u**(-3)) - 0.873251073806898/u)**0.333333333333333)</t>
+          <t>0.0346431827680954</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>1.388620689655172</v>
+        <v>15.86413793103448</v>
       </c>
       <c r="D98" t="n">
         <v>0.55</v>
@@ -2008,14 +2008,14 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>-2.53710396943526*(sqrt(0.00028355401359331/u**2 + u**(-3)) - 0.0168390621352055/u)**0.333333333333333 + 2.53710396943526/(u*(sqrt(0.00028355401359331/u**2 + u**(-3)) - 0.0168390621352055/u)**0.333333333333333)</t>
+          <t>0.00517840704548767</t>
         </is>
       </c>
       <c r="C99" t="n">
         <v>19.31068965517241</v>
       </c>
       <c r="D99" t="n">
-        <v>0.55</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="100">
@@ -2024,14 +2024,14 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>-0.960423757048652*(sqrt(0.0336456842739398/u**2 + u**(-3)) - 0.183427599542544/u)**0.333333333333333 + 0.960423757048652/(u*(sqrt(0.0336456842739398/u**2 + u**(-3)) - 0.183427599542544/u)**0.333333333333333)</t>
+          <t>0.192146083167879</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>2.767241379310344</v>
+        <v>4.835172413793103</v>
       </c>
       <c r="D100" t="n">
-        <v>0.325</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
@@ -2040,14 +2040,14 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>-2.34900321241884*(sqrt(0.000893802879488867/u**2 + u**(-3)) - 0.0298965362456735/u)**0.333333333333333 + 2.34900321241884/(u*(sqrt(0.000893802879488867/u**2 + u**(-3)) - 0.0298965362456735/u)**0.333333333333333)</t>
+          <t>0.00557650464339154</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>16.55344827586207</v>
+        <v>17.93206896551724</v>
       </c>
       <c r="D101" t="n">
-        <v>0.775</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="102">
@@ -2056,14 +2056,14 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>-1.35701667376402*(sqrt(0.0400339926650359/u**2 + u**(-3)) - 0.20008496361555/u)**0.333333333333333 + 1.35701667376402/(u*(sqrt(0.0400339926650359/u**2 + u**(-3)) - 0.20008496361555/u)**0.333333333333333)</t>
+          <t>0.121813617516276</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>5.524482758620689</v>
+        <v>6.213793103448275</v>
       </c>
       <c r="D102" t="n">
-        <v>1</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="103">
@@ -2072,14 +2072,14 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>-2.34900321241884*(sqrt(0.00015718281647619/u**2 + u**(-3)) - 0.0125372571352824/u)**0.333333333333333 + 2.34900321241884/(u*(sqrt(0.00015718281647619/u**2 + u**(-3)) - 0.0125372571352824/u)**0.333333333333333)</t>
+          <t>0.00604090421857340</t>
         </is>
       </c>
       <c r="C103" t="n">
         <v>16.55344827586207</v>
       </c>
       <c r="D103" t="n">
-        <v>0.325</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="104">
@@ -2088,11 +2088,11 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>-2.03450126623181*(sqrt(0.00211736449709364/u**2 + u**(-3)) - 0.0460148290999069/u)**0.333333333333333 + 2.03450126623181/(u*(sqrt(0.00211736449709364/u**2 + u**(-3)) - 0.0460148290999069/u)**0.333333333333333)</t>
+          <t>0.110323182252287</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>12.41758620689655</v>
+        <v>6.903103448275861</v>
       </c>
       <c r="D104" t="n">
         <v>0.775</v>
@@ -2104,14 +2104,14 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>-2.44486325217569*(sqrt(0.000354109803579031/u**2 + u**(-3)) - 0.0188178054931767/u)**0.333333333333333 + 2.44486325217569/(u*(sqrt(0.000354109803579031/u**2 + u**(-3)) - 0.0188178054931767/u)**0.333333333333333)</t>
+          <t>0.0797008021098380</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>17.93206896551724</v>
+        <v>9.660344827586206</v>
       </c>
       <c r="D105" t="n">
-        <v>0.55</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="106">
@@ -2120,14 +2120,14 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>-2.09020705128496*(sqrt(0.00299781037098507/u**2 + u**(-3)) - 0.05475226361517/u)**0.333333333333333 + 2.09020705128496/(u*(sqrt(0.00299781037098507/u**2 + u**(-3)) - 0.05475226361517/u)**0.333333333333333)</t>
+          <t>0.0666047168092996</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>13.10689655172414</v>
+        <v>4.835172413793103</v>
       </c>
       <c r="D106" t="n">
-        <v>1</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="107">
@@ -2136,14 +2136,14 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>-2.14446628142853*(sqrt(0.00257054183757931/u**2 + u**(-3)) - 0.0507005112161536/u)**0.333333333333333 + 2.14446628142853/(u*(sqrt(0.00257054183757931/u**2 + u**(-3)) - 0.0507005112161536/u)**0.333333333333333)</t>
+          <t>0.0188446110210699</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>13.79620689655172</v>
+        <v>17.24275862068966</v>
       </c>
       <c r="D107" t="n">
-        <v>1</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="108">
@@ -2152,14 +2152,14 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>-0.729049867913356*(sqrt(u**(-2) + 0.660455737430731/u**3) - 1/u)**0.333333333333333 + 0.634899728523648/(u*(sqrt(u**(-2) + 0.660455737430731/u**3) - 1/u)**0.333333333333333)</t>
+          <t>0.216669713378737</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>1.388620689655172</v>
+        <v>4.145862068965517</v>
       </c>
       <c r="D108" t="n">
-        <v>0.775</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
@@ -2168,11 +2168,11 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>-1.35701667376402*(sqrt(0.0240454168444372/u**2 + u**(-3)) - 0.155065846802051/u)**0.333333333333333 + 1.35701667376402/(u*(sqrt(0.0240454168444372/u**2 + u**(-3)) - 0.155065846802051/u)**0.333333333333333)</t>
+          <t>0.0589726985878816</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>5.524482758620689</v>
+        <v>13.10689655172414</v>
       </c>
       <c r="D109" t="n">
         <v>0.775</v>
@@ -2184,14 +2184,14 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>-1.72926135317545*(sqrt(0.00282814435951592/u**2 + u**(-3)) - 0.0531803004835054/u)**0.333333333333333 + 1.72926135317546/(u*(sqrt(0.00282814435951592/u**2 + u**(-3)) - 0.0531803004835054/u)**0.333333333333333)</t>
+          <t>0.0144818383369635</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>8.97103448275862</v>
+        <v>6.903103448275861</v>
       </c>
       <c r="D110" t="n">
-        <v>0.55</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="111">
@@ -2200,14 +2200,14 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>-2.14446628142853*(sqrt(0.000777588905867743/u**2 + u**(-3)) - 0.0278852811688845/u)**0.333333333333333 + 2.14446628142853/(u*(sqrt(0.000777588905867743/u**2 + u**(-3)) - 0.0278852811688845/u)**0.333333333333333)</t>
+          <t>0.463440739406359</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>13.79620689655172</v>
+        <v>0.01</v>
       </c>
       <c r="D111" t="n">
-        <v>0.55</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
@@ -2216,14 +2216,14 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>-1.51691610933453*(sqrt(0.0205196820814356/u**2 + u**(-3)) - 0.143246926952852/u)**0.333333333333333 + 1.51691610933453/(u*(sqrt(0.0205196820814356/u**2 + u**(-3)) - 0.143246926952852/u)**0.333333333333333)</t>
+          <t>0.0288610174857200</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>6.903103448275861</v>
+        <v>3.45655172413793</v>
       </c>
       <c r="D112" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="113">
@@ -2232,14 +2232,14 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>-1.43918878810811*(sqrt(0.000281341246048555/u**2 + u**(-3)) - 0.0167732300421998/u)**0.333333333333333 + 1.43918878810811/(u*(sqrt(0.000281341246048555/u**2 + u**(-3)) - 0.0167732300421998/u)**0.333333333333333)</t>
+          <t>0.0361749367898064</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>6.213793103448275</v>
+        <v>8.97103448275862</v>
       </c>
       <c r="D113" t="n">
-        <v>0.1</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="114">
@@ -2248,14 +2248,14 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>-2.39741239816944*(sqrt(0.00131668996912629/u**2 + u**(-3)) - 0.0362862228556003/u)**0.333333333333333 + 2.39741239816944/(u*(sqrt(0.00131668996912629/u**2 + u**(-3)) - 0.0362862228556003/u)**0.333333333333333)</t>
+          <t>0.0247844907285102</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>17.24275862068966</v>
+        <v>13.10689655172414</v>
       </c>
       <c r="D114" t="n">
-        <v>1</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="115">
@@ -2264,14 +2264,14 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>-2.44486325217569*(sqrt(0.00117061092092242/u**2 + u**(-3)) - 0.0342141918057758/u)**0.333333333333333 + 2.44486325217569/(u*(sqrt(0.00117061092092242/u**2 + u**(-3)) - 0.0342141918057758/u)**0.333333333333333)</t>
+          <t>0.00762923236606450</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>17.93206896551724</v>
+        <v>13.10689655172414</v>
       </c>
       <c r="D115" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="116">
@@ -2280,11 +2280,11 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>-2.14446628142853*(sqrt(0.000271513481594315/u**2 + u**(-3)) - 0.0164776661452499/u)**0.333333333333333 + 2.14446628142853/(u*(sqrt(0.000271513481594315/u**2 + u**(-3)) - 0.0164776661452499/u)**0.333333333333333)</t>
+          <t>0.0294181015400687</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>13.79620689655172</v>
+        <v>11.03896551724138</v>
       </c>
       <c r="D116" t="n">
         <v>0.325</v>
@@ -2296,11 +2296,11 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>-1.91824273031694*(sqrt(5.01786118392806e-5/u**2 + u**(-3)) - 0.00708368631711488/u)**0.333333333333333 + 1.91824273031694/(u*(sqrt(5.01786118392806e-5/u**2 + u**(-3)) - 0.00708368631711488/u)**0.333333333333333)</t>
+          <t>0.0476055831738185</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>11.03896551724138</v>
+        <v>2.077931034482758</v>
       </c>
       <c r="D117" t="n">
         <v>0.1</v>
@@ -2312,14 +2312,14 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>-1.59085027507341*(sqrt(0.000154228332961269/u**2 + u**(-3)) - 0.0124188700356059/u)**0.333333333333333 + 1.59085027507341/(u*(sqrt(0.000154228332961269/u**2 + u**(-3)) - 0.0124188700356059/u)**0.333333333333333)</t>
+          <t>0.102404338016511</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>7.592413793103447</v>
+        <v>9.660344827586206</v>
       </c>
       <c r="D118" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
@@ -2328,11 +2328,11 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>-2.24906110678856*(sqrt(1.93166796126826e-5/u**2 + u**(-3)) - 0.00439507447180166/u)**0.333333333333333 + 2.24906110678856/(u*(sqrt(1.93166796126826e-5/u**2 + u**(-3)) - 0.00439507447180166/u)**0.333333333333333)</t>
+          <t>0.00499993750234373</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>15.1748275862069</v>
+        <v>20</v>
       </c>
       <c r="D119" t="n">
         <v>0.1</v>
@@ -2344,14 +2344,14 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>-1.17556540566168*(sqrt(0.0286539569583753/u**2 + u**(-3)) - 0.169274797174226/u)**0.333333333333333 + 1.17556540566168/(u*(sqrt(0.0286539569583753/u**2 + u**(-3)) - 0.169274797174226/u)**0.333333333333333)</t>
+          <t>0.0584672552709218</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>4.145862068965517</v>
+        <v>5.524482758620689</v>
       </c>
       <c r="D120" t="n">
-        <v>0.55</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="121">
@@ -2360,14 +2360,14 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>-1.07339829888349*(sqrt(0.16344611138971/u**2 + u**(-3)) - 0.404284691015762/u)**0.333333333333333 + 1.07339829888349/(u*(sqrt(0.16344611138971/u**2 + u**(-3)) - 0.404284691015762/u)**0.333333333333333)</t>
+          <t>0.273985833231339</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>3.45655172413793</v>
+        <v>2.077931034482758</v>
       </c>
       <c r="D121" t="n">
-        <v>1</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="122">
@@ -2376,14 +2376,14 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>-1.07339829888349*(sqrt(0.0016344611138971/u**2 + u**(-3)) - 0.0404284691015762/u)**0.333333333333333 + 1.07339829888349/(u*(sqrt(0.0016344611138971/u**2 + u**(-3)) - 0.0404284691015762/u)**0.333333333333333)</t>
+          <t>0.263829420217390</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>3.45655172413793</v>
+        <v>1.388620689655172</v>
       </c>
       <c r="D122" t="n">
-        <v>0.1</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="123">
@@ -2392,14 +2392,14 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>-1.97722666564972*(sqrt(0.00251307043146634/u**2 + u**(-3)) - 0.0501305339236113/u)**0.333333333333333 + 1.97722666564972/(u*(sqrt(0.00251307043146634/u**2 + u**(-3)) - 0.0501305339236113/u)**0.333333333333333)</t>
+          <t>0.0529980358164615</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>11.72827586206896</v>
+        <v>10.34965517241379</v>
       </c>
       <c r="D123" t="n">
-        <v>0.775</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="124">
@@ -2408,14 +2408,14 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>-0.482807879260335*(sqrt(0.197375805112653/u**2 + u**(-3)) - 0.444269968726959/u)**0.333333333333333 + 0.482807879260335/(u*(sqrt(0.197375805112653/u**2 + u**(-3)) - 0.444269968726959/u)**0.333333333333333)</t>
+          <t>0.379418735800452</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>0.6993103448275861</v>
+        <v>0.01</v>
       </c>
       <c r="D124" t="n">
-        <v>0.1</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="125">
@@ -2424,14 +2424,14 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>-2.39741239816944*(sqrt(0.000398298715660702/u**2 + u**(-3)) - 0.0199574225705802/u)**0.333333333333333 + 2.39741239816944/(u*(sqrt(0.000398298715660702/u**2 + u**(-3)) - 0.0199574225705802/u)**0.333333333333333)</t>
+          <t>0.0560472452474874</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>17.24275862068966</v>
+        <v>13.79620689655172</v>
       </c>
       <c r="D125" t="n">
-        <v>0.55</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="126">
@@ -2440,14 +2440,14 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>-0.7937005259841*(sqrt(u**(-2) + 0.0506647711673295/u**3) - 1/u)**0.333333333333333 + 0.293691941285839/(u*(sqrt(u**(-2) + 0.0506647711673295/u**3) - 1/u)**0.333333333333333)</t>
+          <t>0.100729437244842</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>0.6993103448275861</v>
+        <v>7.592413793103447</v>
       </c>
       <c r="D126" t="n">
-        <v>1</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="127">
@@ -2456,14 +2456,14 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>-0.680348119140775*(sqrt(0.266268382243653/u**2 + u**(-3)) - 0.516011998158621/u)**0.333333333333333 + 0.680348119140775/(u*(sqrt(0.266268382243653/u**2 + u**(-3)) - 0.516011998158621/u)**0.333333333333333)</t>
+          <t>0.0497122179435829</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>1.388620689655172</v>
+        <v>11.03896551724138</v>
       </c>
       <c r="D127" t="n">
-        <v>0.325</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="128">
@@ -2472,14 +2472,14 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>-2.24906110678856*(sqrt(0.00116020806923675/u**2 + u**(-3)) - 0.0340618271564629/u)**0.333333333333333 + 2.24906110678856/(u*(sqrt(0.00116020806923675/u**2 + u**(-3)) - 0.0340618271564629/u)**0.333333333333333)</t>
+          <t>0.0660631494860881</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>15.1748275862069</v>
+        <v>8.281724137931034</v>
       </c>
       <c r="D128" t="n">
-        <v>0.775</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="129">
@@ -2488,14 +2488,14 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>-1.51691610933453*(sqrt(0.00620720382963428/u**2 + u**(-3)) - 0.0787858098240684/u)**0.333333333333333 + 1.51691610933453/(u*(sqrt(0.00620720382963428/u**2 + u**(-3)) - 0.0787858098240684/u)**0.333333333333333)</t>
+          <t>0.0722107644039857</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>6.903103448275861</v>
+        <v>13.79620689655172</v>
       </c>
       <c r="D129" t="n">
-        <v>0.55</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130">
@@ -2504,14 +2504,14 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>-2.19738611698682*(sqrt(0.00133384435674143/u**2 + u**(-3)) - 0.0365218339728638/u)**0.333333333333333 + 2.19738611698682/(u*(sqrt(0.00133384435674143/u**2 + u**(-3)) - 0.0365218339728638/u)**0.333333333333333)</t>
+          <t>0.0917871527876128</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>14.48551724137931</v>
+        <v>3.45655172413793</v>
       </c>
       <c r="D130" t="n">
-        <v>0.775</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="131">
@@ -2520,14 +2520,14 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>-2.19738611698682*(sqrt(0.00222076063557366/u**2 + u**(-3)) - 0.0471249470617598/u)**0.333333333333333 + 2.19738611698682/(u*(sqrt(0.00222076063557366/u**2 + u**(-3)) - 0.0471249470617598/u)**0.333333333333333)</t>
+          <t>0.00852587402216265</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>14.48551724137931</v>
+        <v>11.72827586206896</v>
       </c>
       <c r="D131" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="132">
@@ -2536,14 +2536,14 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>-2.09020705128496*(sqrt(2.99781037098507e-5/u**2 + u**(-3)) - 0.00547522636151701/u)**0.333333333333333 + 2.09020705128496/(u*(sqrt(2.99781037098507e-5/u**2 + u**(-3)) - 0.00547522636151701/u)**0.333333333333333)</t>
+          <t>0.0520757229946654</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>13.10689655172414</v>
+        <v>6.213793103448275</v>
       </c>
       <c r="D132" t="n">
-        <v>0.1</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="133">
@@ -2552,14 +2552,14 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>-2.39741239816944*(sqrt(1.31668996912629e-5/u**2 + u**(-3)) - 0.00362862228556003/u)**0.333333333333333 + 2.39741239816944/(u*(sqrt(1.31668996912629e-5/u**2 + u**(-3)) - 0.00362862228556003/u)**0.333333333333333)</t>
+          <t>0.0214105794147534</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>17.24275862068966</v>
+        <v>15.1748275862069</v>
       </c>
       <c r="D133" t="n">
-        <v>0.1</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="134">
@@ -2568,14 +2568,14 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>-0.368403149864039*(sqrt(u**(-2) + 1.48148148148148e-5/u**3) - 1/u)**0.333333333333333 + 0.00904805872198302/(u*(sqrt(u**(-2) + 1.48148148148148e-5/u**3) - 1/u)**0.333333333333333)</t>
+          <t>0.0162478553415615</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>0.01</v>
+        <v>20</v>
       </c>
       <c r="D134" t="n">
-        <v>0.1</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="135">
@@ -2584,14 +2584,14 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>-0.729049867913356*(sqrt(u**(-2) + 2.46656646240413e-7/u**3) - 1/u)**0.333333333333333 + 0.0045721609454149/(u*(sqrt(u**(-2) + 2.46656646240413e-7/u**3) - 1/u)**0.333333333333333)</t>
+          <t>0.128890218111263</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>0.01</v>
+        <v>7.592413793103447</v>
       </c>
       <c r="D135" t="n">
-        <v>0.775</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136">
@@ -2600,14 +2600,14 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>-1.97722666564972*(sqrt(0.00418409228964219/u**2 + u**(-3)) - 0.0646845599014339/u)**0.333333333333333 + 1.97722666564972/(u*(sqrt(0.00418409228964219/u**2 + u**(-3)) - 0.0646845599014339/u)**0.333333333333333)</t>
+          <t>0.0695872644114314</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>11.72827586206896</v>
+        <v>1.388620689655172</v>
       </c>
       <c r="D136" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="137">
@@ -2616,14 +2616,14 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>-1.26953697777222*(sqrt(0.0358650370002738/u**2 + u**(-3)) - 0.189380666912634/u)**0.333333333333333 + 1.26953697777222/(u*(sqrt(0.0358650370002738/u**2 + u**(-3)) - 0.189380666912634/u)**0.333333333333333)</t>
+          <t>0.0789611349741056</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>4.835172413793103</v>
+        <v>6.903103448275861</v>
       </c>
       <c r="D137" t="n">
-        <v>0.775</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="138">
@@ -2632,14 +2632,14 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>-2.58198889747161*(sqrt(8.912109375e-5/u**2 + u**(-3)) - 0.00944039690638058/u)**0.333333333333333 + 2.58198889747161/(u*(sqrt(8.912109375e-5/u**2 + u**(-3)) - 0.00944039690638058/u)**0.333333333333333)</t>
+          <t>0.216112104285731</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>20</v>
+        <v>2.077931034482758</v>
       </c>
       <c r="D138" t="n">
-        <v>0.325</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="139">
@@ -2648,14 +2648,14 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>-0.7937005259841*(sqrt(u**(-2) + 0.396686227294333/u**3) - 1/u)**0.333333333333333 + 0.583184145738696/(u*(sqrt(u**(-2) + 0.396686227294333/u**3) - 1/u)**0.333333333333333)</t>
+          <t>0.00630336775641926</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>1.388620689655172</v>
+        <v>15.86413793103448</v>
       </c>
       <c r="D139" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="140">
@@ -2664,11 +2664,11 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>-0.7937005259841*(sqrt(u**(-2) + 1.48148148148148e-7/u**3) - 1/u)**0.333333333333333 + 0.00419973683298291/(u*(sqrt(u**(-2) + 1.48148148148148e-7/u**3) - 1/u)**0.333333333333333)</t>
+          <t>0.140817330330892</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>0.01</v>
+        <v>6.903103448275861</v>
       </c>
       <c r="D140" t="n">
         <v>1</v>
@@ -2680,11 +2680,11 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>-1.79446787169031*(sqrt(0.000790847248685053/u**2 + u**(-3)) - 0.0281220064839807/u)**0.333333333333333 + 1.79446787169031/(u*(sqrt(0.000790847248685053/u**2 + u**(-3)) - 0.0281220064839807/u)**0.333333333333333)</t>
+          <t>0.186973703454270</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>9.660344827586206</v>
+        <v>1.388620689655172</v>
       </c>
       <c r="D141" t="n">
         <v>0.325</v>
@@ -2696,14 +2696,14 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>-1.43918878810811*(sqrt(0.00297166691138786/u**2 + u**(-3)) - 0.0545129976371495/u)**0.333333333333333 + 1.43918878810811/(u*(sqrt(0.00297166691138786/u**2 + u**(-3)) - 0.0545129976371495/u)**0.333333333333333)</t>
+          <t>0.0103504495089122</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>6.213793103448275</v>
+        <v>9.660344827586206</v>
       </c>
       <c r="D142" t="n">
-        <v>0.325</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="143">
@@ -2712,14 +2712,14 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>-1.07339829888349*(sqrt(0.0494424486953874/u**2 + u**(-3)) - 0.222356580058669/u)**0.333333333333333 + 1.07339829888349/(u*(sqrt(0.0494424486953874/u**2 + u**(-3)) - 0.222356580058669/u)**0.333333333333333)</t>
+          <t>0.0517131742590532</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>3.45655172413793</v>
+        <v>19.31068965517241</v>
       </c>
       <c r="D143" t="n">
-        <v>0.55</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
@@ -2728,14 +2728,14 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>-0.960423757048652*(sqrt(0.191322500516309/u**2 + u**(-3)) - 0.43740427583222/u)**0.333333333333333 + 0.960423757048652/(u*(sqrt(0.191322500516309/u**2 + u**(-3)) - 0.43740427583222/u)**0.333333333333333)</t>
+          <t>0.0174502037167701</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>2.767241379310344</v>
+        <v>18.62137931034483</v>
       </c>
       <c r="D144" t="n">
-        <v>0.775</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="145">
@@ -2744,11 +2744,11 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>-2.44486325217569*(sqrt(0.00012364577852243/u**2 + u**(-3)) - 0.0111196123368771/u)**0.333333333333333 + 2.44486325217569/(u*(sqrt(0.00012364577852243/u**2 + u**(-3)) - 0.0111196123368771/u)**0.333333333333333)</t>
+          <t>0.0336034126771529</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>17.93206896551724</v>
+        <v>9.660344827586206</v>
       </c>
       <c r="D145" t="n">
         <v>0.325</v>
@@ -2760,14 +2760,14 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>-1.35701667376402*(sqrt(0.00422859047524441/u**2 + u**(-3)) - 0.0650276131750537/u)**0.333333333333333 + 1.35701667376402/(u*(sqrt(0.00422859047524441/u**2 + u**(-3)) - 0.0650276131750537/u)**0.333333333333333)</t>
+          <t>0.109986737387342</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>5.524482758620689</v>
+        <v>8.97103448275862</v>
       </c>
       <c r="D146" t="n">
-        <v>0.325</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147">
@@ -2776,11 +2776,11 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>-2.29957517315949*(sqrt(1.69065246187952e-5/u**2 + u**(-3)) - 0.00411175444534267/u)**0.333333333333333 + 2.29957517315949/(u*(sqrt(1.69065246187952e-5/u**2 + u**(-3)) - 0.00411175444534267/u)**0.333333333333333)</t>
+          <t>0.118938144118934</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>15.86413793103448</v>
+        <v>0.6993103448275861</v>
       </c>
       <c r="D147" t="n">
         <v>0.1</v>
@@ -2792,11 +2792,11 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>-2.53710396943526*(sqrt(0.000563007039386717/u**2 + u**(-3)) - 0.023727769372335/u)**0.333333333333333 + 2.53710396943526/(u*(sqrt(0.000563007039386717/u**2 + u**(-3)) - 0.023727769372335/u)**0.333333333333333)</t>
+          <t>0.320662947470474</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>19.31068965517241</v>
+        <v>1.388620689655172</v>
       </c>
       <c r="D148" t="n">
         <v>0.775</v>
@@ -2808,14 +2808,14 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>-2.29957517315949*(sqrt(0.00169065246187952/u**2 + u**(-3)) - 0.0411175444534267/u)**0.333333333333333 + 2.29957517315949/(u*(sqrt(0.00169065246187952/u**2 + u**(-3)) - 0.0411175444534267/u)**0.333333333333333)</t>
+          <t>0.0387209725573782</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>15.86413793103448</v>
+        <v>20</v>
       </c>
       <c r="D149" t="n">
-        <v>1</v>
+        <v>0.775</v>
       </c>
     </row>
     <row r="150">
@@ -2824,14 +2824,14 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>-2.19738611698682*(sqrt(0.000671780092261033/u**2 + u**(-3)) - 0.0259187208839679/u)**0.333333333333333 + 2.19738611698682/(u*(sqrt(0.000671780092261033/u**2 + u**(-3)) - 0.0259187208839679/u)**0.333333333333333)</t>
+          <t>0.0391704664589533</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>14.48551724137931</v>
+        <v>8.281724137931034</v>
       </c>
       <c r="D150" t="n">
-        <v>0.55</v>
+        <v>0.325</v>
       </c>
     </row>
     <row r="151">
@@ -2840,14 +2840,14 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>-2.09020705128496*(sqrt(0.000906837637222985/u**2 + u**(-3)) - 0.0301137449883435/u)**0.333333333333333 + 2.09020705128496/(u*(sqrt(0.000906837637222985/u**2 + u**(-3)) - 0.0301137449883435/u)**0.333333333333333)</t>
+          <t>0.0120726557124948</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>13.10689655172414</v>
+        <v>8.281724137931034</v>
       </c>
       <c r="D151" t="n">
-        <v>0.55</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>